<commit_message>
Updated test cases with bad examples
</commit_message>
<xml_diff>
--- a/DataTable.xlsx
+++ b/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsiddiqsunny/Documents/Notre Dame/Research/SecurityEval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262004E3-F1D0-E048-B137-9DCD33886EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130070B8-4D81-234E-B704-FC6D35324525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{E3FB6B4D-BFE5-BF42-BAE6-66D1841BF3B8}"/>
   </bookViews>
@@ -542,10 +542,13 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -624,7 +627,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -651,7 +654,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -659,7 +662,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -672,7 +675,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -686,7 +689,7 @@
         <v>36</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -695,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -705,7 +708,7 @@
         <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -722,11 +725,11 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>3</v>

</xml_diff>